<commit_message>
Flash in Quad mode works ok
</commit_message>
<xml_diff>
--- a/IR_PCB_hw/Factory/BOM_18-10-2023.xlsx
+++ b/IR_PCB_hw/Factory/BOM_18-10-2023.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Nute\PresentTime\IR_PCB\IR_PCB_hw\Factory\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E30594DD-B937-49E7-8805-25847BE63276}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE92EE3C-6BAF-46F6-AF8A-96AB6C542110}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="134">
   <si>
     <t>Designator</t>
   </si>
@@ -405,18 +405,53 @@
   </si>
   <si>
     <t>Components w/o LEDs etc.</t>
+  </si>
+  <si>
+    <t>Статус</t>
+  </si>
+  <si>
+    <t>Заказано на Али, едет</t>
+  </si>
+  <si>
+    <t>Есть на первую партию</t>
+  </si>
+  <si>
+    <t>Есть</t>
+  </si>
+  <si>
+    <t>Надо заказать где-нибудь (не проблема)</t>
+  </si>
+  <si>
+    <t>Надо заказать неясно где</t>
+  </si>
+  <si>
+    <t>Заказано в Онэлек, едет</t>
+  </si>
+  <si>
+    <t>Заказано в Промэлектронике, едет</t>
+  </si>
+  <si>
+    <t>НАДО НАЙТИ</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -450,8 +485,16 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -485,8 +528,49 @@
         <fgColor rgb="FFFFCC99"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="7">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -566,34 +650,86 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="4" xfId="4"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="9"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="8"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="10"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="8" xfId="4" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="7" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" xfId="11"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="6"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="7"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="5"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="12">
+    <cellStyle name="20% - Accent2" xfId="6" builtinId="34"/>
+    <cellStyle name="20% - Accent3" xfId="8" builtinId="38"/>
+    <cellStyle name="40% - Accent2" xfId="7" builtinId="35"/>
+    <cellStyle name="40% - Accent3" xfId="9" builtinId="39"/>
+    <cellStyle name="40% - Accent4" xfId="11" builtinId="43"/>
+    <cellStyle name="60% - Accent3" xfId="10" builtinId="40"/>
+    <cellStyle name="Bad" xfId="5" builtinId="27"/>
     <cellStyle name="Good" xfId="2" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Input" xfId="4" builtinId="20"/>
@@ -934,21 +1070,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K34"/>
+  <dimension ref="A1:L34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H34" sqref="H34"/>
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.7109375" customWidth="1"/>
-    <col min="2" max="4" width="15.7109375" customWidth="1"/>
-    <col min="5" max="5" width="25.7109375" customWidth="1"/>
-    <col min="6" max="10" width="12.7109375" customWidth="1"/>
+    <col min="1" max="1" width="36.7109375" style="2" customWidth="1"/>
+    <col min="2" max="4" width="15.7109375" style="11" customWidth="1"/>
+    <col min="5" max="5" width="25.7109375" style="11" customWidth="1"/>
+    <col min="6" max="10" width="12.7109375" style="11" customWidth="1"/>
+    <col min="11" max="11" width="9.140625" style="11"/>
+    <col min="12" max="12" width="38.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -982,946 +1120,978 @@
       <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L1" s="8" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="2">
+      <c r="H2" s="11">
         <v>1</v>
       </c>
-      <c r="I2" s="2">
+      <c r="I2" s="11">
         <v>11</v>
       </c>
-      <c r="J2" s="2">
+      <c r="J2" s="11">
         <v>11</v>
       </c>
-      <c r="K2" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K2" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="L2" s="18" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="H3" s="2">
+      <c r="H3" s="11">
         <v>1</v>
       </c>
-      <c r="I3" s="2">
+      <c r="I3" s="11">
         <v>15</v>
       </c>
-      <c r="J3" s="2">
+      <c r="J3" s="11">
         <v>15</v>
       </c>
-      <c r="K3" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K3" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="L3" s="10" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="G4" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="H4" s="2">
+      <c r="H4" s="11">
         <v>12</v>
       </c>
-      <c r="I4" s="2">
+      <c r="I4" s="11">
         <v>0.17</v>
       </c>
-      <c r="J4" s="2">
+      <c r="J4" s="11">
         <v>2.04</v>
       </c>
-      <c r="K4" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K4" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="L4" s="9" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F5" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="G5" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="H5" s="2">
+      <c r="H5" s="11">
         <v>1</v>
       </c>
-      <c r="I5" s="2">
+      <c r="I5" s="11">
         <v>1.51</v>
       </c>
-      <c r="J5" s="2">
+      <c r="J5" s="11">
         <v>1.51</v>
       </c>
-      <c r="K5" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K5" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="L5" s="9" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E6" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F6" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="G6" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="H6" s="2">
+      <c r="H6" s="11">
         <v>2</v>
       </c>
-      <c r="I6" s="2">
+      <c r="I6" s="11">
         <v>0.48</v>
       </c>
-      <c r="J6" s="2">
+      <c r="J6" s="11">
         <v>0.96</v>
       </c>
-      <c r="K6" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K6" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="L6" s="9" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E7" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="F7" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="G7" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="H7" s="2">
+      <c r="H7" s="11">
         <v>2</v>
       </c>
-      <c r="I7" s="2">
+      <c r="I7" s="11">
         <v>0.23</v>
       </c>
-      <c r="J7" s="2">
+      <c r="J7" s="11">
         <v>0.46</v>
       </c>
-      <c r="K7" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K7" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="L7" s="9" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E8" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="F8" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="G8" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="H8" s="2">
+      <c r="H8" s="11">
         <v>4</v>
       </c>
-      <c r="I8" s="2">
+      <c r="I8" s="11">
         <v>1.52</v>
       </c>
-      <c r="J8" s="2">
+      <c r="J8" s="11">
         <v>6.08</v>
       </c>
-      <c r="K8" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K8" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="L8" s="9" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="E9" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="F9" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="G9" s="2" t="s">
+      <c r="G9" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="H9" s="2">
+      <c r="H9" s="11">
         <v>3</v>
       </c>
-      <c r="I9" s="2">
+      <c r="I9" s="11">
         <v>5.04</v>
       </c>
-      <c r="J9" s="2">
+      <c r="J9" s="11">
         <v>15.12</v>
       </c>
-      <c r="K9" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K9" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="L9" s="19" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2" t="s">
+      <c r="E10" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2">
+      <c r="H10" s="11">
         <v>1</v>
       </c>
-      <c r="I10" s="2">
+      <c r="I10" s="11">
         <v>12.59</v>
       </c>
-      <c r="J10" s="2">
+      <c r="J10" s="11">
         <v>12.59</v>
       </c>
-      <c r="K10" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K10" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="L10" s="20" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D11" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="E11" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2">
+      <c r="H11" s="11">
         <v>1</v>
       </c>
-      <c r="I11" s="2">
+      <c r="I11" s="11">
         <v>3.46</v>
       </c>
-      <c r="J11" s="2">
+      <c r="J11" s="11">
         <v>3.46</v>
       </c>
-      <c r="K11" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K11" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="L11" s="9" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2" t="s">
+      <c r="E12" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2">
-        <v>10</v>
-      </c>
-      <c r="I12" s="2">
+      <c r="H12" s="11">
+        <v>10</v>
+      </c>
+      <c r="I12" s="11">
         <v>4.5</v>
       </c>
-      <c r="J12" s="2">
+      <c r="J12" s="11">
         <v>45</v>
       </c>
-      <c r="K12" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K12" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="L12" s="19" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D13" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="E13" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2">
+      <c r="H13" s="11">
         <v>1</v>
       </c>
-      <c r="I13" s="2">
+      <c r="I13" s="11">
         <v>10.59</v>
       </c>
-      <c r="J13" s="2">
+      <c r="J13" s="11">
         <v>10.59</v>
       </c>
-      <c r="K13" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K13" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="L13" s="7" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2" t="s">
+      <c r="C14" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D14" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="E14" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2">
+      <c r="H14" s="11">
         <v>1</v>
       </c>
-      <c r="I14" s="2">
+      <c r="I14" s="11">
         <v>16.149999999999999</v>
       </c>
-      <c r="J14" s="2">
+      <c r="J14" s="11">
         <v>16.149999999999999</v>
       </c>
-      <c r="K14" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K14" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="L14" s="10" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2" t="s">
+      <c r="C15" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2" t="s">
+      <c r="E15" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2">
+      <c r="H15" s="11">
         <v>1</v>
       </c>
-      <c r="I15" s="2">
+      <c r="I15" s="11">
         <v>15.89</v>
       </c>
-      <c r="J15" s="2">
+      <c r="J15" s="11">
         <v>15.89</v>
       </c>
-      <c r="K15" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K15" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="L15" s="19" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2" t="s">
+      <c r="C16" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2" t="s">
+      <c r="E16" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2">
+      <c r="H16" s="11">
         <v>1</v>
       </c>
-      <c r="I16" s="2">
+      <c r="I16" s="11">
         <v>109.59</v>
       </c>
-      <c r="J16" s="2">
+      <c r="J16" s="11">
         <v>109.59</v>
       </c>
-      <c r="K16" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K16" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="L16" s="7" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2" t="s">
+      <c r="C17" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="D17" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="E17" s="2" t="s">
+      <c r="E17" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2">
+      <c r="H17" s="11">
         <v>1</v>
       </c>
-      <c r="I17" s="2">
+      <c r="I17" s="11">
         <v>26.65</v>
       </c>
-      <c r="J17" s="2">
+      <c r="J17" s="11">
         <v>26.65</v>
       </c>
-      <c r="K17" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K17" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="L17" s="19" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2" t="s">
+      <c r="C18" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="D18" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="E18" s="2" t="s">
+      <c r="E18" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2">
+      <c r="H18" s="11">
         <v>1</v>
       </c>
-      <c r="I18" s="2">
+      <c r="I18" s="11">
         <v>42.63</v>
       </c>
-      <c r="J18" s="2">
+      <c r="J18" s="11">
         <v>42.63</v>
       </c>
-      <c r="K18" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K18" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="L18" s="18" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C19" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="D19" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="E19" s="2" t="s">
+      <c r="E19" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2" t="s">
+      <c r="G19" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="H19" s="2">
+      <c r="H19" s="11">
         <v>1</v>
       </c>
-      <c r="I19" s="2">
+      <c r="I19" s="11">
         <v>0.85</v>
       </c>
-      <c r="J19" s="2">
+      <c r="J19" s="11">
         <v>0.85</v>
       </c>
-      <c r="K19" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K19" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="L19" s="9" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2" t="s">
+      <c r="C20" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2" t="s">
+      <c r="E20" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2">
+      <c r="H20" s="11">
         <v>2</v>
       </c>
-      <c r="I20" s="2">
+      <c r="I20" s="11">
         <v>3</v>
       </c>
-      <c r="J20" s="2">
+      <c r="J20" s="11">
         <v>6</v>
       </c>
-      <c r="K20" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K20" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="L20" s="19" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2" t="s">
+      <c r="C21" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2" t="s">
+      <c r="E21" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
-      <c r="H21" s="2">
+      <c r="H21" s="11">
         <v>3</v>
       </c>
-      <c r="I21" s="2">
+      <c r="I21" s="11">
         <v>80.2</v>
       </c>
-      <c r="J21" s="2">
+      <c r="J21" s="11">
         <v>240.6</v>
       </c>
-      <c r="K21" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K21" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="L21" s="21" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2" t="s">
+      <c r="C22" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2" t="s">
+      <c r="E22" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2" t="s">
+      <c r="G22" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="H22" s="2">
+      <c r="H22" s="11">
         <v>6</v>
       </c>
-      <c r="I22" s="2">
+      <c r="I22" s="11">
         <v>4</v>
       </c>
-      <c r="J22" s="2">
+      <c r="J22" s="11">
         <v>24</v>
       </c>
-      <c r="K22" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K22" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="L22" s="19" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B23" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="C23" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="D23" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="E23" s="2" t="s">
+      <c r="E23" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2" t="s">
+      <c r="G23" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="H23" s="2">
+      <c r="H23" s="11">
         <v>8</v>
       </c>
-      <c r="I23" s="2">
+      <c r="I23" s="11">
         <v>0.2</v>
       </c>
-      <c r="J23" s="2">
+      <c r="J23" s="11">
         <v>1.6</v>
       </c>
-      <c r="K23" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K23" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="L23" s="9" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B24" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="C24" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="D24" s="2" t="s">
+      <c r="D24" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="E24" s="2" t="s">
+      <c r="E24" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="F24" s="2"/>
-      <c r="G24" s="2" t="s">
+      <c r="G24" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="H24" s="2">
+      <c r="H24" s="11">
         <v>2</v>
       </c>
-      <c r="I24" s="2">
+      <c r="I24" s="11">
         <v>0.31</v>
       </c>
-      <c r="J24" s="2">
+      <c r="J24" s="11">
         <v>0.62</v>
       </c>
-      <c r="K24" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K24" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="L24" s="9" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B25" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="C25" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="D25" s="2" t="s">
+      <c r="D25" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="E25" s="2" t="s">
+      <c r="E25" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="F25" s="2"/>
-      <c r="G25" s="2" t="s">
+      <c r="G25" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="H25" s="2">
+      <c r="H25" s="11">
         <v>4</v>
       </c>
-      <c r="I25" s="2">
+      <c r="I25" s="11">
         <v>0.11</v>
       </c>
-      <c r="J25" s="2">
+      <c r="J25" s="11">
         <v>0.44</v>
       </c>
-      <c r="K25" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K25" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="L25" s="9" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B26" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="C26" s="11" t="s">
         <v>106</v>
       </c>
-      <c r="D26" s="2" t="s">
+      <c r="D26" s="11" t="s">
         <v>107</v>
       </c>
-      <c r="E26" s="2" t="s">
+      <c r="E26" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="F26" s="2"/>
-      <c r="G26" s="2" t="s">
+      <c r="G26" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="H26" s="2">
+      <c r="H26" s="11">
         <v>1</v>
       </c>
-      <c r="I26" s="2">
+      <c r="I26" s="11">
         <v>0.15</v>
       </c>
-      <c r="J26" s="2">
+      <c r="J26" s="11">
         <v>0.15</v>
       </c>
-      <c r="K26" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K26" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="L26" s="19" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B27" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="C27" s="11" t="s">
         <v>109</v>
       </c>
-      <c r="D27" s="2" t="s">
+      <c r="D27" s="11" t="s">
         <v>110</v>
       </c>
-      <c r="E27" s="2" t="s">
+      <c r="E27" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="F27" s="2"/>
-      <c r="G27" s="2" t="s">
+      <c r="G27" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="H27" s="2">
-        <v>10</v>
-      </c>
-      <c r="I27" s="2">
+      <c r="H27" s="11">
+        <v>10</v>
+      </c>
+      <c r="I27" s="11">
         <v>0.26</v>
       </c>
-      <c r="J27" s="2">
+      <c r="J27" s="11">
         <v>2.6</v>
       </c>
-      <c r="K27" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K27" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="L27" s="9" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B28" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="C28" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="D28" s="2" t="s">
+      <c r="D28" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="E28" s="2" t="s">
+      <c r="E28" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="F28" s="2"/>
-      <c r="G28" s="2" t="s">
+      <c r="G28" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="H28" s="2">
+      <c r="H28" s="11">
         <v>3</v>
       </c>
-      <c r="I28" s="2">
+      <c r="I28" s="11">
         <v>0.35</v>
       </c>
-      <c r="J28" s="2">
+      <c r="J28" s="11">
         <v>1.05</v>
       </c>
-      <c r="K28" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K28" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="L28" s="9" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="B29" s="2"/>
-      <c r="C29" s="2" t="s">
+      <c r="C29" s="11" t="s">
         <v>115</v>
       </c>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2" t="s">
+      <c r="E29" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="F29" s="2"/>
-      <c r="G29" s="2"/>
-      <c r="H29" s="2">
+      <c r="H29" s="11">
         <v>1</v>
       </c>
-      <c r="I29" s="2">
+      <c r="I29" s="11">
         <v>40</v>
       </c>
-      <c r="J29" s="2">
+      <c r="J29" s="11">
         <v>40</v>
       </c>
-      <c r="K29" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="6" t="s">
+      <c r="K29" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="L29" s="7" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="B30" s="6"/>
-      <c r="C30" s="6" t="s">
+      <c r="B30" s="12"/>
+      <c r="C30" s="12" t="s">
         <v>118</v>
       </c>
-      <c r="D30" s="6" t="s">
+      <c r="D30" s="12" t="s">
         <v>119</v>
       </c>
-      <c r="E30" s="6" t="s">
+      <c r="E30" s="12" t="s">
         <v>120</v>
       </c>
-      <c r="F30" s="6"/>
-      <c r="G30" s="6"/>
-      <c r="H30" s="6">
+      <c r="F30" s="12"/>
+      <c r="G30" s="12"/>
+      <c r="H30" s="12">
         <v>1</v>
       </c>
-      <c r="I30" s="6">
+      <c r="I30" s="12">
         <v>11.26</v>
       </c>
-      <c r="J30" s="6">
+      <c r="J30" s="12">
         <v>11.26</v>
       </c>
-      <c r="K30" s="7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="9" t="s">
+      <c r="K30" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="L30" s="19" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="B31" s="10"/>
-      <c r="C31" s="10"/>
-      <c r="D31" s="10"/>
-      <c r="E31" s="10"/>
-      <c r="F31" s="10"/>
-      <c r="G31" s="10"/>
-      <c r="H31" s="10">
+      <c r="B31" s="13"/>
+      <c r="C31" s="13"/>
+      <c r="D31" s="13"/>
+      <c r="E31" s="13"/>
+      <c r="F31" s="13"/>
+      <c r="G31" s="13"/>
+      <c r="H31" s="13">
         <v>1</v>
       </c>
-      <c r="I31" s="10">
+      <c r="I31" s="13">
         <v>146.15</v>
       </c>
-      <c r="J31" s="10">
+      <c r="J31" s="13">
         <f>I31*H31</f>
         <v>146.15</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H32" s="11" t="s">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H32" s="14" t="s">
         <v>123</v>
       </c>
-      <c r="I32" s="11"/>
-      <c r="J32" s="11">
+      <c r="I32" s="14"/>
+      <c r="J32" s="14">
         <f>SUM(J2:J30)</f>
         <v>663.8900000000001</v>
       </c>
     </row>
     <row r="33" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="H33" s="5" t="s">
+      <c r="H33" s="15" t="s">
         <v>124</v>
       </c>
-      <c r="I33" s="5"/>
-      <c r="J33" s="5">
+      <c r="I33" s="15"/>
+      <c r="J33" s="15">
         <f>J32-J12-J21</f>
         <v>378.29000000000008</v>
       </c>
     </row>
     <row r="34" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="I34" s="4" t="s">
+      <c r="I34" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="J34" s="4">
+      <c r="J34" s="3">
         <f>SUM(J2:J31)</f>
         <v>810.04000000000008</v>
       </c>

</xml_diff>